<commit_message>
ja com bue informação
</commit_message>
<xml_diff>
--- a/Reprografias.xlsx
+++ b/Reprografias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\CoimbraInk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\projetos\CoimbraInk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078F493B-F1A8-478E-95CB-6382E6224383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825F893D-6F6E-40B1-9FA5-A39AE93EE1AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4E3E08FD-BF37-48D8-952B-5250572D8340}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E3E08FD-BF37-48D8-952B-5250572D8340}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="221">
   <si>
     <t>Latitude</t>
   </si>
@@ -550,6 +550,150 @@
   </si>
   <si>
     <t>40.204160</t>
+  </si>
+  <si>
+    <t>Teste Hugo</t>
+  </si>
+  <si>
+    <t>Alberto</t>
+  </si>
+  <si>
+    <t>40.21231</t>
+  </si>
+  <si>
+    <t>www.alberto.com</t>
+  </si>
+  <si>
+    <t>hugo@alberto.com</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>23.00</t>
+  </si>
+  <si>
+    <t>9.50</t>
+  </si>
+  <si>
+    <t>12.50</t>
+  </si>
+  <si>
+    <t>14.50</t>
+  </si>
+  <si>
+    <t>23.50</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>0.32</t>
+  </si>
+  <si>
+    <t>0.321</t>
+  </si>
+  <si>
+    <t>0.890</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>0.3213</t>
+  </si>
+  <si>
+    <t>0.21312</t>
+  </si>
+  <si>
+    <t>0.3232</t>
+  </si>
+  <si>
+    <t>0.32132131</t>
+  </si>
+  <si>
+    <t>0.832</t>
+  </si>
+  <si>
+    <t>0.9555</t>
+  </si>
+  <si>
+    <t>0.83232</t>
+  </si>
+  <si>
+    <t>0.9123</t>
+  </si>
+  <si>
+    <t>0.732</t>
+  </si>
+  <si>
+    <t>0.323</t>
+  </si>
+  <si>
+    <t>0.3254</t>
+  </si>
+  <si>
+    <t>0.4354</t>
+  </si>
+  <si>
+    <t>0.465</t>
+  </si>
+  <si>
+    <t>0.5463</t>
+  </si>
+  <si>
+    <t>0.5465</t>
+  </si>
+  <si>
+    <t>0.564645</t>
+  </si>
+  <si>
+    <t>0.431321</t>
+  </si>
+  <si>
+    <t>0.213112</t>
+  </si>
+  <si>
+    <t>0.321312</t>
+  </si>
+  <si>
+    <t>0.32131</t>
+  </si>
+  <si>
+    <t>0.5334</t>
+  </si>
+  <si>
+    <t>0.534</t>
+  </si>
+  <si>
+    <t>0.535</t>
+  </si>
+  <si>
+    <t>0.543</t>
+  </si>
+  <si>
+    <t>0.321321</t>
+  </si>
+  <si>
+    <t>0.3211</t>
   </si>
 </sst>
 </file>
@@ -624,7 +768,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -641,7 +785,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -939,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D278AB-7120-4BE3-B8B1-9FE1A4C04DD2}">
   <dimension ref="A1:BH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BC29" sqref="BC29:BC30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4646,7 +4790,183 @@
       </c>
     </row>
     <row r="21" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="BG21" s="3"/>
+      <c r="A21" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D21" s="3">
+        <v>-8.4212321321899992</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F21" s="3">
+        <v>935877377</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="X21" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y21" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z21" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA21" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AB21" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="AC21" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD21" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE21" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="AF21" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="AG21" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AH21" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AI21" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AJ21" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AK21" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AL21" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AM21" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="AN21" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="AO21" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="AP21" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="AQ21" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="AR21" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="AS21" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AT21" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="AU21" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="AV21" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AW21" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="AX21" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="AY21" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="AZ21" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="BA21" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BB21" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="BC21" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BD21" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="BE21" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="BF21" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="BG21" s="3">
+        <v>5</v>
+      </c>
       <c r="BH21" s="3"/>
     </row>
   </sheetData>
@@ -4661,8 +4981,10 @@
     <hyperlink ref="E11" r:id="rId8" xr:uid="{65FA1AC9-BEFC-4D92-B61A-51CFE5578CAF}"/>
     <hyperlink ref="G11" r:id="rId9" xr:uid="{454D9B3B-A1C0-4F46-BA0A-6B8916437E8B}"/>
     <hyperlink ref="G7" r:id="rId10" xr:uid="{6D51CB25-8392-4DFB-8A62-9699BFEE2C0C}"/>
+    <hyperlink ref="E21" r:id="rId11" xr:uid="{18B6A34D-57EC-4A9D-B757-EFAA4EC0D173}"/>
+    <hyperlink ref="G21" r:id="rId12" xr:uid="{6D2908D8-6A06-4205-B978-5FE58AE12476}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reprografias e horario fixed
</commit_message>
<xml_diff>
--- a/Reprografias.xlsx
+++ b/Reprografias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\projetos\CoimbraInk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08610EE0-83C6-4B32-B918-4889EBB8BA1E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF02BC1D-1785-4F23-A36D-7BA33E362C59}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E3E08FD-BF37-48D8-952B-5250572D8340}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="217">
   <si>
     <t>Latitude</t>
   </si>
@@ -679,6 +679,9 @@
   </si>
   <si>
     <t>0.3211</t>
+  </si>
+  <si>
+    <t>10.30</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1072,7 @@
   <dimension ref="A1:BH19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3161,17 +3164,17 @@
       <c r="H12" s="3">
         <v>0</v>
       </c>
-      <c r="I12" s="3">
-        <v>-1</v>
-      </c>
-      <c r="J12" s="3">
-        <v>-1</v>
+      <c r="I12" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="K12" s="3">
-        <v>-1</v>
+        <v>15</v>
       </c>
       <c r="L12" s="3">
-        <v>-1</v>
+        <v>17</v>
       </c>
       <c r="M12" s="3">
         <v>-1</v>

</xml_diff>

<commit_message>
adicionei o horario ao fds e corrigi um bug na base de dados, apaguem e insiram
</commit_message>
<xml_diff>
--- a/Reprografias.xlsx
+++ b/Reprografias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\projetos\CoimbraInk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF02BC1D-1785-4F23-A36D-7BA33E362C59}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37476AB5-5C18-4F8F-90ED-595829A1B137}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E3E08FD-BF37-48D8-952B-5250572D8340}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="216">
   <si>
     <t>Latitude</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>Horario Fecho Semana Tarde</t>
-  </si>
-  <si>
-    <t>13-30</t>
   </si>
   <si>
     <t>MundiCópia</t>
@@ -1072,7 +1069,7 @@
   <dimension ref="A1:BH19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,130 +1186,130 @@
         <v>13</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="BG1" s="2" t="s">
         <v>14</v>
@@ -1329,7 +1326,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D2" s="3">
         <v>-8.4154060000000008</v>
@@ -1392,115 +1389,115 @@
         <v>-1</v>
       </c>
       <c r="X2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB2">
+        <v>-1</v>
+      </c>
+      <c r="AC2">
+        <v>-1</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF2" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="Y2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AG2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH2" t="s">
         <v>107</v>
       </c>
-      <c r="AA2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB2">
-        <v>-1</v>
-      </c>
-      <c r="AC2">
-        <v>-1</v>
-      </c>
-      <c r="AD2" t="s">
+      <c r="AI2">
+        <v>-1</v>
+      </c>
+      <c r="AJ2">
+        <v>-1</v>
+      </c>
+      <c r="AK2" t="s">
         <v>114</v>
       </c>
-      <c r="AE2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AI2">
-        <v>-1</v>
-      </c>
-      <c r="AJ2">
-        <v>-1</v>
-      </c>
-      <c r="AK2" t="s">
+      <c r="AL2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AM2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AN2">
+        <v>-1</v>
+      </c>
+      <c r="AO2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AP2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AQ2">
+        <v>-1</v>
+      </c>
+      <c r="AR2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AS2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AT2">
+        <v>-1</v>
+      </c>
+      <c r="AU2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AV2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AW2">
+        <v>-1</v>
+      </c>
+      <c r="AX2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AY2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AZ2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BA2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BB2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BC2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BD2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BE2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BF2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BG2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BH2" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="AL2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AM2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AN2">
-        <v>-1</v>
-      </c>
-      <c r="AO2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AP2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AQ2">
-        <v>-1</v>
-      </c>
-      <c r="AR2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AS2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AT2">
-        <v>-1</v>
-      </c>
-      <c r="AU2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AV2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AW2">
-        <v>-1</v>
-      </c>
-      <c r="AX2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AY2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AZ2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BA2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BB2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BC2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BD2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BE2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BF2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BG2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BH2" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.25">
@@ -1511,7 +1508,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D3" s="3">
         <v>-8.4101189999999999</v>
@@ -1574,115 +1571,115 @@
         <v>-1</v>
       </c>
       <c r="X3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB3">
+        <v>-1</v>
+      </c>
+      <c r="AC3">
+        <v>-1</v>
+      </c>
+      <c r="AD3">
+        <v>-1</v>
+      </c>
+      <c r="AE3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="Y3" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB3">
-        <v>-1</v>
-      </c>
-      <c r="AC3">
-        <v>-1</v>
-      </c>
-      <c r="AD3">
-        <v>-1</v>
-      </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AF3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI3">
+        <v>-1</v>
+      </c>
+      <c r="AJ3">
+        <v>-1</v>
+      </c>
+      <c r="AK3">
+        <v>-1</v>
+      </c>
+      <c r="AL3" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AM3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AN3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AO3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AP3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AQ3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AR3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AS3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AT3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AU3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AV3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AW3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AX3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AY3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AZ3" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BA3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="BB3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="BC3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="BD3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="BE3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="BF3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="BG3" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BH3" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="AF3" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>118</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>107</v>
-      </c>
-      <c r="AI3">
-        <v>-1</v>
-      </c>
-      <c r="AJ3">
-        <v>-1</v>
-      </c>
-      <c r="AK3">
-        <v>-1</v>
-      </c>
-      <c r="AL3" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AM3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="AN3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="AO3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="AP3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="AQ3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="AR3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="AS3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="AT3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="AU3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="AV3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="AW3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="AX3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="AY3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="AZ3" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BA3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="BB3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="BC3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="BD3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="BE3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="BF3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="BG3" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BH3" s="5" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:60" ht="30" x14ac:dyDescent="0.25">
@@ -1693,7 +1690,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D4" s="3">
         <v>-8.4124990000000004</v>
@@ -1756,10 +1753,10 @@
         <v>-1</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Z4">
         <v>-1</v>
@@ -1771,16 +1768,16 @@
         <v>-1</v>
       </c>
       <c r="AC4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD4" s="3">
         <v>-1</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AG4">
         <v>-1</v>
@@ -1792,7 +1789,7 @@
         <v>-1</v>
       </c>
       <c r="AJ4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AK4">
         <v>-1</v>
@@ -1864,7 +1861,7 @@
         <v>-1</v>
       </c>
       <c r="BH4" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:60" ht="30" x14ac:dyDescent="0.25">
@@ -1875,7 +1872,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D5" s="3">
         <v>-8.4152539999999991</v>
@@ -1938,31 +1935,31 @@
         <v>-1</v>
       </c>
       <c r="X5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y5" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="Y5" s="3" t="s">
+      <c r="Z5" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AE5" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="Z5" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AA5" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AB5" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AC5" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AD5" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AE5" s="3" t="s">
+      <c r="AF5" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="AF5" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="AG5" s="3">
         <v>-1</v>
@@ -2049,13 +2046,13 @@
     </row>
     <row r="6" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D6" s="3">
         <v>-8.4166969999999992</v>
@@ -2118,32 +2115,32 @@
         <v>-1</v>
       </c>
       <c r="X6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AE6" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="Y6" s="3" t="s">
+      <c r="AF6" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="Z6" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AB6" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AC6" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AD6" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="AG6" s="3">
         <v>-1</v>
       </c>
@@ -2226,18 +2223,18 @@
         <v>-1</v>
       </c>
       <c r="BH6" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D7" s="3">
         <v>-8.4125960000000006</v>
@@ -2300,32 +2297,32 @@
         <v>-1</v>
       </c>
       <c r="X7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AE7" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="Y7" s="3" t="s">
+      <c r="AF7" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="Z7" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AA7" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AB7" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AC7" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AD7" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AE7" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AF7" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="AG7" s="3">
         <v>-1</v>
       </c>
@@ -2408,7 +2405,7 @@
         <v>-1</v>
       </c>
       <c r="BH7" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:60" ht="30" x14ac:dyDescent="0.25">
@@ -2419,7 +2416,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8" s="3">
         <v>-8.4180130000000002</v>
@@ -2590,7 +2587,7 @@
         <v>-1</v>
       </c>
       <c r="BH8" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:60" ht="30" x14ac:dyDescent="0.25">
@@ -2601,7 +2598,7 @@
         <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D9" s="3">
         <v>-8.4206710000000005</v>
@@ -2661,34 +2658,34 @@
         <v>-1</v>
       </c>
       <c r="W9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z9">
+        <v>-1</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AC9">
+        <v>-1</v>
+      </c>
+      <c r="AD9" t="s">
         <v>130</v>
       </c>
-      <c r="X9" s="3" t="s">
+      <c r="AE9" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="Y9" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z9">
-        <v>-1</v>
-      </c>
-      <c r="AA9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AB9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AC9">
-        <v>-1</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>131</v>
-      </c>
-      <c r="AE9" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="AF9" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AG9">
         <v>-1</v>
@@ -2703,7 +2700,7 @@
         <v>-1</v>
       </c>
       <c r="AK9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AL9" s="3">
         <v>-1</v>
@@ -2724,66 +2721,66 @@
         <v>2</v>
       </c>
       <c r="AR9" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AT9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AU9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AV9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AW9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AX9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BA9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BB9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BC9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BD9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BE9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BF9" t="s">
+        <v>130</v>
+      </c>
+      <c r="BG9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BH9" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="AS9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AT9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AU9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AV9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AW9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AX9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AY9" t="s">
-        <v>131</v>
-      </c>
-      <c r="AZ9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BA9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BB9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BC9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BD9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BE9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BF9" t="s">
-        <v>131</v>
-      </c>
-      <c r="BG9" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BH9" s="3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D10" s="3">
         <v>-8.4235389999999999</v>
@@ -2846,32 +2843,32 @@
         <v>-1</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Y10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AC10">
+        <v>-1</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AE10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF10" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="Z10" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB10" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AC10">
-        <v>-1</v>
-      </c>
-      <c r="AD10" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AE10" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF10" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="AG10" s="3">
         <v>-1</v>
       </c>
@@ -2954,7 +2951,7 @@
         <v>-1</v>
       </c>
       <c r="BH10" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:60" ht="30" x14ac:dyDescent="0.25">
@@ -2965,7 +2962,7 @@
         <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D11" s="3">
         <v>-8.4252289999999999</v>
@@ -3028,126 +3025,126 @@
         <v>-1</v>
       </c>
       <c r="X11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AE11" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF11" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG11">
+        <v>-1</v>
+      </c>
+      <c r="AH11">
+        <v>-1</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AJ11" t="s">
         <v>107</v>
       </c>
-      <c r="Y11" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AA11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AB11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AE11" s="3" t="s">
+      <c r="AK11">
+        <v>-1</v>
+      </c>
+      <c r="AL11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AM11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AN11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AO11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AP11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AQ11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AR11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AS11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AT11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AU11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AV11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AW11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AX11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AY11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AZ11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BA11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BB11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BC11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BD11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BE11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BF11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BG11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BH11" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="AF11" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG11">
-        <v>-1</v>
-      </c>
-      <c r="AH11">
-        <v>-1</v>
-      </c>
-      <c r="AI11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>108</v>
-      </c>
-      <c r="AK11">
-        <v>-1</v>
-      </c>
-      <c r="AL11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AM11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AN11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AO11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AP11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AQ11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AR11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AS11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AT11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AU11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AV11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AW11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AX11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AY11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AZ11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BA11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BB11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BC11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BD11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BE11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BF11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BG11" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BH11" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D12" s="3">
         <v>-8.4229430000000001</v>
@@ -3165,7 +3162,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>31</v>
@@ -3210,32 +3207,32 @@
         <v>-1</v>
       </c>
       <c r="X12" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AE12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="Y12" s="3" t="s">
+      <c r="AF12" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="Z12" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AA12" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AB12" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AC12" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AD12" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AE12" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AF12" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="AG12" s="3">
         <v>-1</v>
       </c>
@@ -3318,7 +3315,7 @@
         <v>-1</v>
       </c>
       <c r="BH12" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:60" ht="30" x14ac:dyDescent="0.25">
@@ -3329,7 +3326,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D13" s="3">
         <v>-8.420909</v>
@@ -3392,115 +3389,115 @@
         <v>-1</v>
       </c>
       <c r="X13" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Y13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AE13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AF13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AG13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AH13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AI13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AJ13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AK13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AL13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AM13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AN13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AO13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AP13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AQ13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AR13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AS13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AT13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AU13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AV13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AW13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AX13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AY13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AZ13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BA13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BB13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BC13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BD13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BE13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BF13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BG13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BH13" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="Z13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AA13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AB13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AE13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AF13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AG13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AH13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AI13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AJ13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AK13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AL13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AM13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AN13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AO13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AP13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AQ13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AR13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AS13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AT13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AU13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AV13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AW13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AX13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AY13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AZ13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BA13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BB13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BC13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BD13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BE13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BF13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BG13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BH13" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:60" x14ac:dyDescent="0.25">
@@ -3511,7 +3508,7 @@
         <v>52</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D14" s="6">
         <v>-8.4029330000000009</v>
@@ -3693,7 +3690,7 @@
         <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D15" s="3">
         <v>-8.4084070000000004</v>
@@ -3872,10 +3869,10 @@
         <v>57</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D16" s="3">
         <v>-8.4076140000000006</v>
@@ -4054,10 +4051,10 @@
         <v>60</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D17" s="3">
         <v>-8.4049420000000001</v>
@@ -4090,7 +4087,7 @@
         <v>10</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="O17" s="3">
         <v>14</v>
@@ -4120,126 +4117,126 @@
         <v>-1</v>
       </c>
       <c r="X17" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AE17" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF17" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="Y17" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AA17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AB17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AC17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AD17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AE17" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="AF17" s="3" t="s">
+      <c r="AG17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AH17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AI17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AJ17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AK17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AL17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AM17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AN17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AO17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AP17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AQ17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AR17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AS17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AT17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AU17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AV17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AW17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AX17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AY17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AZ17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BA17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BB17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BC17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BD17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BE17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BF17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BG17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BH17" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="AG17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AH17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AI17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AJ17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AK17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AL17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AM17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AN17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AO17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AP17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AQ17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AR17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AS17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AT17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AU17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AV17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AW17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AX17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AY17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AZ17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BA17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BB17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BC17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BD17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BE17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BF17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BG17" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BH17" s="3" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D18" s="3">
         <v>-8.4026700000000005</v>
@@ -4251,7 +4248,7 @@
         <v>917238155</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H18" s="3">
         <v>0</v>
@@ -4302,10 +4299,10 @@
         <v>-1</v>
       </c>
       <c r="X18" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y18" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Z18" s="3">
         <v>-1</v>
@@ -4317,126 +4314,126 @@
         <v>-1</v>
       </c>
       <c r="AC18" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD18" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE18" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG18">
+        <v>-1</v>
+      </c>
+      <c r="AH18">
+        <v>-1</v>
+      </c>
+      <c r="AI18">
+        <v>-1</v>
+      </c>
+      <c r="AJ18" t="s">
         <v>144</v>
       </c>
-      <c r="AD18" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE18" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="AF18" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG18">
-        <v>-1</v>
-      </c>
-      <c r="AH18">
-        <v>-1</v>
-      </c>
-      <c r="AI18">
-        <v>-1</v>
-      </c>
-      <c r="AJ18" t="s">
+      <c r="AK18" t="s">
+        <v>130</v>
+      </c>
+      <c r="AL18" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AM18" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AN18">
+        <v>-1</v>
+      </c>
+      <c r="AO18">
+        <v>-1</v>
+      </c>
+      <c r="AP18">
+        <v>-1</v>
+      </c>
+      <c r="AQ18">
+        <v>-1</v>
+      </c>
+      <c r="AR18">
+        <v>-1</v>
+      </c>
+      <c r="AS18">
+        <v>-1</v>
+      </c>
+      <c r="AT18">
+        <v>-1</v>
+      </c>
+      <c r="AU18">
+        <v>-1</v>
+      </c>
+      <c r="AV18">
+        <v>-1</v>
+      </c>
+      <c r="AW18">
+        <v>-1</v>
+      </c>
+      <c r="AX18">
+        <v>-1</v>
+      </c>
+      <c r="AY18">
+        <v>-1</v>
+      </c>
+      <c r="AZ18" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BA18" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BB18">
+        <v>-1</v>
+      </c>
+      <c r="BC18">
+        <v>-1</v>
+      </c>
+      <c r="BD18">
+        <v>-1</v>
+      </c>
+      <c r="BE18">
+        <v>-1</v>
+      </c>
+      <c r="BF18">
+        <v>-1</v>
+      </c>
+      <c r="BG18" s="3">
+        <v>-1</v>
+      </c>
+      <c r="BH18" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="AK18" t="s">
-        <v>131</v>
-      </c>
-      <c r="AL18" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AM18" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AN18">
-        <v>-1</v>
-      </c>
-      <c r="AO18">
-        <v>-1</v>
-      </c>
-      <c r="AP18">
-        <v>-1</v>
-      </c>
-      <c r="AQ18">
-        <v>-1</v>
-      </c>
-      <c r="AR18">
-        <v>-1</v>
-      </c>
-      <c r="AS18">
-        <v>-1</v>
-      </c>
-      <c r="AT18">
-        <v>-1</v>
-      </c>
-      <c r="AU18">
-        <v>-1</v>
-      </c>
-      <c r="AV18">
-        <v>-1</v>
-      </c>
-      <c r="AW18">
-        <v>-1</v>
-      </c>
-      <c r="AX18">
-        <v>-1</v>
-      </c>
-      <c r="AY18">
-        <v>-1</v>
-      </c>
-      <c r="AZ18" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BA18" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BB18">
-        <v>-1</v>
-      </c>
-      <c r="BC18">
-        <v>-1</v>
-      </c>
-      <c r="BD18">
-        <v>-1</v>
-      </c>
-      <c r="BE18">
-        <v>-1</v>
-      </c>
-      <c r="BF18">
-        <v>-1</v>
-      </c>
-      <c r="BG18" s="3">
-        <v>-1</v>
-      </c>
-      <c r="BH18" s="3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="D19" s="3">
         <v>-8.4212321321899992</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F19" s="3">
         <v>935877377</v>
       </c>
       <c r="G19" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>22</v>
@@ -4448,145 +4445,145 @@
         <v>45</v>
       </c>
       <c r="L19" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="M19" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="M19" s="3" t="s">
+      <c r="N19" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="N19" s="3" t="s">
+      <c r="O19" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="O19" s="3" t="s">
+      <c r="P19" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="P19" s="3" t="s">
+      <c r="Q19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="R19" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="Q19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="R19" s="3" t="s">
+      <c r="S19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="T19" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="S19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="T19" s="3" t="s">
+      <c r="U19" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="U19" s="3" t="s">
+      <c r="V19" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="V19" s="3" t="s">
+      <c r="W19" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="W19" s="3" t="s">
+      <c r="X19" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="X19" s="3" t="s">
+      <c r="Y19" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z19" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="Y19" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="Z19" s="3" t="s">
+      <c r="AA19" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="AA19" s="3" t="s">
+      <c r="AB19" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="AB19" s="3" t="s">
+      <c r="AC19" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="AC19" s="3" t="s">
+      <c r="AD19" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="AD19" s="3" t="s">
+      <c r="AE19" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="AE19" s="3" t="s">
+      <c r="AF19" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="AF19" s="3" t="s">
+      <c r="AG19" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="AG19" s="3" t="s">
+      <c r="AH19" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AI19" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="AH19" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="AI19" s="3" t="s">
+      <c r="AJ19" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="AJ19" s="3" t="s">
+      <c r="AK19" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="AK19" s="3" t="s">
+      <c r="AL19" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="AL19" s="3" t="s">
+      <c r="AM19" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="AM19" s="3" t="s">
+      <c r="AN19" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="AN19" s="3" t="s">
+      <c r="AO19" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="AO19" s="3" t="s">
+      <c r="AP19" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="AP19" s="3" t="s">
+      <c r="AQ19" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR19" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="AQ19" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AR19" s="3" t="s">
+      <c r="AS19" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="AS19" s="3" t="s">
+      <c r="AT19" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="AT19" s="3" t="s">
+      <c r="AU19" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="AU19" s="3" t="s">
+      <c r="AV19" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="AV19" s="3" t="s">
+      <c r="AW19" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="AW19" s="3" t="s">
+      <c r="AX19" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="AX19" s="3" t="s">
+      <c r="AY19" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="AY19" s="3" t="s">
+      <c r="AZ19" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="AZ19" s="3" t="s">
+      <c r="BA19" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="BA19" s="3" t="s">
+      <c r="BB19" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BC19" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="BD19" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="BB19" s="3" t="s">
+      <c r="BE19" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="BC19" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="BD19" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="BE19" s="3" t="s">
+      <c r="BF19" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="BF19" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="BG19" s="3">
         <v>5</v>

</xml_diff>

<commit_message>
changes to security and correct inserts
</commit_message>
<xml_diff>
--- a/Reprografias.xlsx
+++ b/Reprografias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\projetos\CoimbraInk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37476AB5-5C18-4F8F-90ED-595829A1B137}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA051EB-4FE0-4688-BA1E-FC078C0651EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E3E08FD-BF37-48D8-952B-5250572D8340}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="168">
   <si>
     <t>Latitude</t>
   </si>
@@ -532,150 +532,6 @@
   </si>
   <si>
     <t>40.204160</t>
-  </si>
-  <si>
-    <t>Teste Hugo</t>
-  </si>
-  <si>
-    <t>Alberto</t>
-  </si>
-  <si>
-    <t>40.21231</t>
-  </si>
-  <si>
-    <t>www.alberto.com</t>
-  </si>
-  <si>
-    <t>hugo@alberto.com</t>
-  </si>
-  <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>23.00</t>
-  </si>
-  <si>
-    <t>9.50</t>
-  </si>
-  <si>
-    <t>12.50</t>
-  </si>
-  <si>
-    <t>14.50</t>
-  </si>
-  <si>
-    <t>23.50</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>0.89</t>
-  </si>
-  <si>
-    <t>0.55</t>
-  </si>
-  <si>
-    <t>0.32</t>
-  </si>
-  <si>
-    <t>0.321</t>
-  </si>
-  <si>
-    <t>0.890</t>
-  </si>
-  <si>
-    <t>0.86</t>
-  </si>
-  <si>
-    <t>0.3213</t>
-  </si>
-  <si>
-    <t>0.21312</t>
-  </si>
-  <si>
-    <t>0.3232</t>
-  </si>
-  <si>
-    <t>0.32132131</t>
-  </si>
-  <si>
-    <t>0.832</t>
-  </si>
-  <si>
-    <t>0.9555</t>
-  </si>
-  <si>
-    <t>0.83232</t>
-  </si>
-  <si>
-    <t>0.9123</t>
-  </si>
-  <si>
-    <t>0.732</t>
-  </si>
-  <si>
-    <t>0.323</t>
-  </si>
-  <si>
-    <t>0.3254</t>
-  </si>
-  <si>
-    <t>0.4354</t>
-  </si>
-  <si>
-    <t>0.465</t>
-  </si>
-  <si>
-    <t>0.5463</t>
-  </si>
-  <si>
-    <t>0.5465</t>
-  </si>
-  <si>
-    <t>0.564645</t>
-  </si>
-  <si>
-    <t>0.431321</t>
-  </si>
-  <si>
-    <t>0.213112</t>
-  </si>
-  <si>
-    <t>0.321312</t>
-  </si>
-  <si>
-    <t>0.32131</t>
-  </si>
-  <si>
-    <t>0.5334</t>
-  </si>
-  <si>
-    <t>0.534</t>
-  </si>
-  <si>
-    <t>0.535</t>
-  </si>
-  <si>
-    <t>0.543</t>
-  </si>
-  <si>
-    <t>0.321321</t>
-  </si>
-  <si>
-    <t>0.3211</t>
   </si>
   <si>
     <t>10.30</t>
@@ -1069,7 +925,7 @@
   <dimension ref="A1:BH19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3162,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>215</v>
+        <v>167</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>31</v>
@@ -4411,183 +4267,41 @@
       </c>
     </row>
     <row r="19" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D19" s="3">
-        <v>-8.4212321321899992</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="F19" s="3">
-        <v>935877377</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="P19" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q19" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="S19" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="T19" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="U19" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="V19" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="W19" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="X19" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="Y19" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z19" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="AA19" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="AB19" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="AC19" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="AD19" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="AE19" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="AF19" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="AG19" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="AH19" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="AI19" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="AJ19" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="AK19" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="AL19" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="AM19" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="AN19" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO19" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="AP19" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="AQ19" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="AR19" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AS19" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="AT19" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="AU19" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AV19" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="AW19" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="AX19" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="AY19" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="AZ19" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="BA19" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="BB19" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="BC19" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="BD19" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="BE19" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="BF19" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="BG19" s="3">
-        <v>5</v>
-      </c>
+      <c r="E19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AG19" s="3"/>
+      <c r="AH19" s="3"/>
+      <c r="AI19" s="3"/>
+      <c r="AJ19" s="3"/>
+      <c r="AK19" s="3"/>
+      <c r="AN19" s="3"/>
+      <c r="AO19" s="3"/>
+      <c r="AP19" s="3"/>
+      <c r="AQ19" s="3"/>
+      <c r="AR19" s="3"/>
+      <c r="AS19" s="3"/>
+      <c r="AT19" s="3"/>
+      <c r="AU19" s="3"/>
+      <c r="AV19" s="3"/>
+      <c r="AW19" s="3"/>
+      <c r="AX19" s="3"/>
+      <c r="AY19" s="3"/>
+      <c r="BB19" s="3"/>
+      <c r="BC19" s="3"/>
+      <c r="BD19" s="3"/>
+      <c r="BE19" s="3"/>
+      <c r="BF19" s="3"/>
+      <c r="BG19" s="3"/>
       <c r="BH19" s="3"/>
     </row>
   </sheetData>
@@ -4602,10 +4316,8 @@
     <hyperlink ref="E10" r:id="rId8" xr:uid="{65FA1AC9-BEFC-4D92-B61A-51CFE5578CAF}"/>
     <hyperlink ref="G10" r:id="rId9" xr:uid="{454D9B3B-A1C0-4F46-BA0A-6B8916437E8B}"/>
     <hyperlink ref="G7" r:id="rId10" xr:uid="{6D51CB25-8392-4DFB-8A62-9699BFEE2C0C}"/>
-    <hyperlink ref="E19" r:id="rId11" xr:uid="{18B6A34D-57EC-4A9D-B757-EFAA4EC0D173}"/>
-    <hyperlink ref="G19" r:id="rId12" xr:uid="{6D2908D8-6A06-4205-B978-5FE58AE12476}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>